<commit_message>
Additional corrections to input data
</commit_message>
<xml_diff>
--- a/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
+++ b/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
@@ -2,37 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\indst\PPRiFUfICaWHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="PPRiFUfICaWHR" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Source:</t>
   </si>
@@ -70,13 +59,70 @@
     <t>other industries</t>
   </si>
   <si>
+    <t>PPRiFUfICaWHR Potential Perc Reduction in Fuel Use from Increased Cogen and Waste Heat Recovery</t>
+  </si>
+  <si>
+    <t>Pot Perc Red in Fuel Use (dimensionless)</t>
+  </si>
+  <si>
+    <t>Waste heat recovery related calculations</t>
+  </si>
+  <si>
+    <t>IEA, WBCSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology Roadmap: Low-Carbon Technology for the Indian Cement Industry </t>
+  </si>
+  <si>
+    <t>https://www.iea.org/publications/freepublications/publication/2012_Cement_in_India_Roadmap.pdf</t>
+  </si>
+  <si>
+    <t>Table 2 Page 15</t>
+  </si>
+  <si>
+    <t>Cogeneration figure</t>
+  </si>
+  <si>
+    <t>IEA</t>
+  </si>
+  <si>
+    <t>Combined Heat and Power</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/publications/freepublications/publication/chp_report.pdf</t>
+  </si>
+  <si>
+    <t>Page 4</t>
+  </si>
+  <si>
+    <t>There was limited information available on this, so a common factor was applied to the sectors for CHP</t>
+  </si>
+  <si>
+    <t>WHR was first only applied to cement and Iron and Steel.</t>
+  </si>
+  <si>
+    <t>More recently, low temperature WHR systems is found to have potential in the fertilizer sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further, AEEE report mentions that technology is not a barrier for WHR uptake, and hence, </t>
+  </si>
+  <si>
+    <t>WHR has been applied to Chemicals sector as well</t>
+  </si>
+  <si>
+    <t>Waste heat recovery</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Clinker</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total demand for energy in 2050 </t>
   </si>
   <si>
-    <t>Cement</t>
-  </si>
-  <si>
-    <t>Clinker</t>
+    <t>Units</t>
   </si>
   <si>
     <t>kWh*1000000</t>
@@ -88,49 +134,16 @@
     <t>Conversion factor (to PJ)</t>
   </si>
   <si>
+    <t>In PJ</t>
+  </si>
+  <si>
+    <t>Total (cement + clinker)</t>
+  </si>
+  <si>
+    <t>Total savings</t>
+  </si>
+  <si>
     <t>Percentage savings</t>
-  </si>
-  <si>
-    <t>Total savings</t>
-  </si>
-  <si>
-    <t>Source: https://www.iea.org/publications/freepublications/publication/chp_report.pdf</t>
-  </si>
-  <si>
-    <t>IEA, WBCSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technology Roadmap: Low-Carbon Technology for the Indian Cement Industry </t>
-  </si>
-  <si>
-    <t>Table 2 Page 15</t>
-  </si>
-  <si>
-    <t>IEA</t>
-  </si>
-  <si>
-    <t>Page 4</t>
-  </si>
-  <si>
-    <t>https://www.iea.org/publications/freepublications/publication/chp_report.pdf</t>
-  </si>
-  <si>
-    <t>https://www.iea.org/publications/freepublications/publication/2012_Cement_in_India_Roadmap.pdf</t>
-  </si>
-  <si>
-    <t>There was limited information available on this, so a common factor was applied to the sectors for CHP</t>
-  </si>
-  <si>
-    <t>Waste heat recovery</t>
-  </si>
-  <si>
-    <t>In PJ</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Total (cement + clinker)</t>
   </si>
   <si>
     <t>Cogeneration</t>
@@ -140,28 +153,7 @@
 year), while in 2030 this saving increases to more than 10% (950 Mt / year) – equivalent to one and a half times India’s total annual emissions of CO2 from power generation. "</t>
   </si>
   <si>
-    <t>Waste heat recovery related calculations</t>
-  </si>
-  <si>
-    <t>Cogeneration figure</t>
-  </si>
-  <si>
-    <t>PPRiFUfICaWHR Potential Perc Reduction in Fuel Use from Increased Cogen and Waste Heat Recovery</t>
-  </si>
-  <si>
-    <t>Combined Heat and Power</t>
-  </si>
-  <si>
-    <t>Sector-wise Investment Potential in WHR for India</t>
-  </si>
-  <si>
-    <t>AEEE, SSEF</t>
-  </si>
-  <si>
-    <t>https://shaktifoundation.in/wp-content/uploads/2017/06/PAT-Pulse-II_May-2016_for-website1.pdf</t>
-  </si>
-  <si>
-    <t>Figure 6, Page 9</t>
+    <t>Source: https://www.iea.org/publications/freepublications/publication/chp_report.pdf</t>
   </si>
   <si>
     <t>Source: https://shaktifoundation.in/wp-content/uploads/2017/06/PAT-Pulse-II_May-2016_for-website1.pdf</t>
@@ -170,49 +162,17 @@
     <t>Page 10</t>
   </si>
   <si>
-    <t>http://knowledgeplatform.in/wp-content/uploads/2016/02/2.-Energy-Savings-in-Ammonia-Urea-Plants-by-FAI.pdf</t>
-  </si>
-  <si>
-    <t>Slide 19</t>
-  </si>
-  <si>
     <t>Page 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further, AEEE report mentions that technology is not a barrier for WHR uptake, and hence, </t>
-  </si>
-  <si>
-    <t>WHR has been applied to Chemicals sector as well</t>
-  </si>
-  <si>
-    <t>Sustainability Outlook - PAT Pulse</t>
-  </si>
-  <si>
-    <t>Fertilizer Association of India</t>
-  </si>
-  <si>
-    <t>Energy Saving Efforts in Indian Ammonian Urea Plants</t>
-  </si>
-  <si>
-    <t>WHR was first only applied to cement and Iron and Steel.</t>
-  </si>
-  <si>
-    <t>More recently, low temperature WHR systems is found to have potential in the fertilizer sector</t>
-  </si>
-  <si>
-    <t>Pot Perc Red in Fuel Use 
-(dimensionless)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,14 +198,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,29 +234,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -315,54 +249,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="12"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="20">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -390,9 +304,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1079500</xdr:rowOff>
+      <xdr:colOff>592137</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>898525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,8 +335,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8445500" y="2082800"/>
-          <a:ext cx="8280400" cy="4152900"/>
+          <a:off x="7972425" y="2841625"/>
+          <a:ext cx="7759700" cy="4210050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -440,9 +354,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1066800</xdr:rowOff>
+      <xdr:colOff>655638</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>885825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -471,8 +385,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="88900" y="2171700"/>
-          <a:ext cx="7988300" cy="4051300"/>
+          <a:off x="88900" y="2933700"/>
+          <a:ext cx="7515225" cy="4105275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -490,7 +404,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>690563</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>76691</xdr:rowOff>
     </xdr:to>
@@ -515,8 +429,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="9058275"/>
-          <a:ext cx="7105650" cy="581516"/>
+          <a:off x="76200" y="8734425"/>
+          <a:ext cx="7562850" cy="552941"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -559,8 +473,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28575" y="10448925"/>
-          <a:ext cx="5248275" cy="2288652"/>
+          <a:off x="28575" y="10058400"/>
+          <a:ext cx="5600700" cy="2174352"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -859,166 +773,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.1328125" customWidth="1"/>
+    <col min="3" max="3" width="29.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>2013</v>
       </c>
-      <c r="G6" s="2">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="11"/>
       <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="G11" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" s="2">
         <v>2008</v>
       </c>
-      <c r="G13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1"/>
     <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1027,21 +901,21 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.3984375" customWidth="1"/>
+    <col min="2" max="2" width="29.3984375" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" customWidth="1"/>
+    <col min="4" max="4" width="38.73046875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1049,168 +923,162 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="10">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="13">
         <f>(780*71+1361*70)/2</f>
         <v>75325</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="13">
         <f>(0.58*780*680*1000+0.58*1361*678*1000)/2</f>
         <v>421415820</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="14">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="15">
         <v>3.6E-9</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="15">
         <v>4.1839999999999999E-12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="10">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="13">
         <f>B4*1000000*3.6/1000000000</f>
         <v>271.17</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="15">
         <f>C4*1000000*4.18/1000000000000</f>
         <v>1761.5181276000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="16">
         <f>B7+C7</f>
         <v>2032.6881276000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="B9">
         <f>(20+30)/2</f>
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>18</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="B10" s="17">
         <f>B9/B8</f>
         <v>1.2298984610845129E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="14"/>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="16">
+        <v>41</v>
+      </c>
+      <c r="B12" s="19">
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-    </row>
-    <row r="34" spans="1:14" ht="95.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:14" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="14"/>
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="14"/>
+      <c r="B14" s="18"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="18"/>
+    </row>
+    <row r="34" spans="1:14" ht="95.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:14" ht="89.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="N39">
         <f>C4*4.18/1000000</f>
         <v>1761.5181275999998</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1219,106 +1087,95 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="23.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7">
-        <f>Data!B12+Data!B10</f>
+      <c r="B2" s="6">
+        <f>Data!B10+Data!B12</f>
         <v>5.2298984610845131E-2</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <f>Data!B12</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
-        <f>Data!B12+Data!B10</f>
+      <c r="B4" s="6">
+        <f>Data!B10+Data!B12</f>
         <v>5.2298984610845131E-2</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
-        <f>Data!B12+Data!B10</f>
+      <c r="B5" s="6">
+        <f>Data!B10+Data!B12</f>
         <v>5.2298984610845131E-2</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f>Data!B12</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>Data!B12</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f>Data!B12</f>
         <v>0.04</v>
       </c>
-      <c r="D9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>